<commit_message>
adding pk and fixing metadatas
</commit_message>
<xml_diff>
--- a/data/raw_data/2025/permits-by-county-2025.xlsx
+++ b/data/raw_data/2025/permits-by-county-2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naughtm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB26C589-1190-43A0-83EE-9AD550AF8DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32472976-728B-47BE-B0D0-539701595FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{711F2E15-F26A-451B-B95B-70CDC9A7A6F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0804BE60-6E3F-46A7-BE5A-4D35DED6C4F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,6 +53,12 @@
     <t>Grand Total</t>
   </si>
   <si>
+    <t>No County Entered</t>
+  </si>
+  <si>
+    <t>Antrim</t>
+  </si>
+  <si>
     <t>Carlow</t>
   </si>
   <si>
@@ -132,12 +138,6 @@
   </si>
   <si>
     <t>Wicklow</t>
-  </si>
-  <si>
-    <t>No County Entered</t>
-  </si>
-  <si>
-    <t>Antrim</t>
   </si>
 </sst>
 </file>
@@ -153,12 +153,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
@@ -166,12 +160,16 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,29 +207,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,443 +562,446 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2FBF4-4443-4927-87BB-258E00D54789}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADC3E56-DC3E-4CE3-9608-72F2228540D6}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7">
-        <v>19903</v>
-      </c>
-      <c r="C3" s="7">
-        <v>2234</v>
-      </c>
-      <c r="D3" s="7">
-        <v>12133</v>
+      <c r="B3" s="8">
+        <v>22542</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2421</v>
+      </c>
+      <c r="D3" s="8">
+        <v>13874</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="7">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7">
+        <v>128</v>
+      </c>
+      <c r="C6" s="7">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7">
+        <v>385</v>
+      </c>
+      <c r="C7" s="7">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7">
+        <v>379</v>
+      </c>
+      <c r="C8" s="7">
+        <v>54</v>
+      </c>
+      <c r="D8" s="7">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2130</v>
+      </c>
+      <c r="C9" s="7">
+        <v>224</v>
+      </c>
+      <c r="D9" s="7">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7">
+        <v>377</v>
+      </c>
+      <c r="C10" s="7">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7">
+        <v>10503</v>
+      </c>
+      <c r="C12" s="7">
+        <v>997</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="7">
+        <v>765</v>
+      </c>
+      <c r="C13" s="7">
+        <v>85</v>
+      </c>
+      <c r="D13" s="7">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7">
+        <v>396</v>
+      </c>
+      <c r="C14" s="7">
+        <v>38</v>
+      </c>
+      <c r="D14" s="7">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="7">
+        <v>914</v>
+      </c>
+      <c r="C15" s="7">
+        <v>139</v>
+      </c>
+      <c r="D15" s="7">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7">
+        <v>405</v>
+      </c>
+      <c r="C16" s="7">
+        <v>33</v>
+      </c>
+      <c r="D16" s="7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="7">
+        <v>170</v>
+      </c>
+      <c r="C17" s="7">
+        <v>50</v>
+      </c>
+      <c r="D17" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="7">
+        <v>68</v>
+      </c>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1164</v>
+      </c>
+      <c r="C19" s="7">
+        <v>123</v>
+      </c>
+      <c r="D19" s="7">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="7">
+        <v>101</v>
+      </c>
+      <c r="C20" s="7">
+        <v>17</v>
+      </c>
+      <c r="D20" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="7">
+        <v>348</v>
+      </c>
+      <c r="C21" s="7">
+        <v>35</v>
+      </c>
+      <c r="D21" s="7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="7">
+        <v>271</v>
+      </c>
+      <c r="C22" s="7">
+        <v>33</v>
+      </c>
+      <c r="D22" s="7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="7">
+        <v>907</v>
+      </c>
+      <c r="C23" s="7">
+        <v>146</v>
+      </c>
+      <c r="D23" s="7">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="7">
+        <v>351</v>
+      </c>
+      <c r="C24" s="7">
+        <v>29</v>
+      </c>
+      <c r="D24" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="7">
+        <v>268</v>
+      </c>
+      <c r="C25" s="7">
+        <v>23</v>
+      </c>
+      <c r="D25" s="7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="7">
+        <v>141</v>
+      </c>
+      <c r="C26" s="7">
+        <v>19</v>
+      </c>
+      <c r="D26" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="7">
+        <v>158</v>
+      </c>
+      <c r="C27" s="7">
+        <v>38</v>
+      </c>
+      <c r="D27" s="7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="7">
+        <v>491</v>
+      </c>
+      <c r="C28" s="7">
+        <v>43</v>
+      </c>
+      <c r="D28" s="7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="7">
+        <v>566</v>
+      </c>
+      <c r="C29" s="7">
+        <v>55</v>
+      </c>
+      <c r="D29" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="7">
+        <v>315</v>
+      </c>
+      <c r="C30" s="7">
+        <v>59</v>
+      </c>
+      <c r="D30" s="7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6">
-        <v>3985</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B31" s="7">
+        <v>565</v>
+      </c>
+      <c r="C31" s="7">
+        <v>41</v>
+      </c>
+      <c r="D31" s="7">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
-        <v>122</v>
-      </c>
-      <c r="C6" s="6">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>301</v>
-      </c>
-      <c r="C7" s="6">
-        <v>33</v>
-      </c>
-      <c r="D7" s="6">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>336</v>
-      </c>
-      <c r="C8" s="6">
-        <v>88</v>
-      </c>
-      <c r="D8" s="6">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1867</v>
-      </c>
-      <c r="C9" s="6">
-        <v>199</v>
-      </c>
-      <c r="D9" s="6">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>309</v>
-      </c>
-      <c r="C10" s="6">
-        <v>45</v>
-      </c>
-      <c r="D10" s="6">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <v>9277</v>
-      </c>
-      <c r="C12" s="6">
-        <v>897</v>
-      </c>
-      <c r="D12" s="6">
-        <v>3249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6">
-        <v>665</v>
-      </c>
-      <c r="C13" s="6">
-        <v>83</v>
-      </c>
-      <c r="D13" s="6">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6">
-        <v>355</v>
-      </c>
-      <c r="C14" s="6">
-        <v>26</v>
-      </c>
-      <c r="D14" s="6">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6">
-        <v>833</v>
-      </c>
-      <c r="C15" s="6">
-        <v>124</v>
-      </c>
-      <c r="D15" s="6">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6">
-        <v>378</v>
-      </c>
-      <c r="C16" s="6">
-        <v>34</v>
-      </c>
-      <c r="D16" s="6">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6">
-        <v>139</v>
-      </c>
-      <c r="C17" s="6">
-        <v>52</v>
-      </c>
-      <c r="D17" s="6">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6">
-        <v>49</v>
-      </c>
-      <c r="C18" s="6">
-        <v>3</v>
-      </c>
-      <c r="D18" s="6">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1023</v>
-      </c>
-      <c r="C19" s="6">
-        <v>113</v>
-      </c>
-      <c r="D19" s="6">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6">
-        <v>90</v>
-      </c>
-      <c r="C20" s="6">
-        <v>15</v>
-      </c>
-      <c r="D20" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6">
-        <v>296</v>
-      </c>
-      <c r="C21" s="6">
-        <v>30</v>
-      </c>
-      <c r="D21" s="6">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6">
-        <v>223</v>
-      </c>
-      <c r="C22" s="6">
-        <v>29</v>
-      </c>
-      <c r="D22" s="6">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6">
-        <v>831</v>
-      </c>
-      <c r="C23" s="6">
-        <v>142</v>
-      </c>
-      <c r="D23" s="6">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6">
-        <v>326</v>
-      </c>
-      <c r="C24" s="6">
+      <c r="B32" s="7">
+        <v>275</v>
+      </c>
+      <c r="C32" s="7">
         <v>27</v>
       </c>
-      <c r="D24" s="6">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6">
-        <v>234</v>
-      </c>
-      <c r="C25" s="6">
-        <v>21</v>
-      </c>
-      <c r="D25" s="6">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6">
-        <v>126</v>
-      </c>
-      <c r="C26" s="6">
-        <v>18</v>
-      </c>
-      <c r="D26" s="6">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6">
-        <v>143</v>
-      </c>
-      <c r="C27" s="6">
-        <v>42</v>
-      </c>
-      <c r="D27" s="6">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6">
-        <v>370</v>
-      </c>
-      <c r="C28" s="6">
-        <v>36</v>
-      </c>
-      <c r="D28" s="6">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6">
-        <v>488</v>
-      </c>
-      <c r="C29" s="6">
-        <v>49</v>
-      </c>
-      <c r="D29" s="6">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6">
-        <v>285</v>
-      </c>
-      <c r="C30" s="6">
-        <v>54</v>
-      </c>
-      <c r="D30" s="6">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6">
-        <v>596</v>
-      </c>
-      <c r="C31" s="6">
-        <v>34</v>
-      </c>
-      <c r="D31" s="6">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6">
-        <v>240</v>
-      </c>
-      <c r="C32" s="6">
-        <v>26</v>
-      </c>
-      <c r="D32" s="6">
-        <v>154</v>
+      <c r="D32" s="7">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1013,62 +1013,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <m02c691f3efa402dab5cbaa8c240a9e7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Statistics</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">9ba6f678-e647-4dac-946a-fcabffeb8025</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">#Reports</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">139e42fd-3e09-4439-bba7-8aeac7f033ff</TermId>
-        </TermInfo>
-      </Terms>
-    </m02c691f3efa402dab5cbaa8c240a9e7>
-    <TaxCatchAll xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Value>8</Value>
-      <Value>5</Value>
-      <Value>10</Value>
-      <Value>1</Value>
-      <Value>7</Value>
-    </TaxCatchAll>
-    <eDocs_FileStatus xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">Live</eDocs_FileStatus>
-    <h1f8bb4843d6459a8b809123185593c7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">218</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d1f665d0-1ea2-48c4-9fae-9dfb881d0110</TermId>
-        </TermInfo>
-      </Terms>
-    </h1f8bb4843d6459a8b809123185593c7>
-    <fbaa881fc4ae443f9fdafbdd527793df xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </fbaa881fc4ae443f9fdafbdd527793df>
-    <_vti_ItemDeclaredRecord xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd" xsi:nil="true"/>
-    <nb1b8a72855341e18dd75ce464e281f2 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2023</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">720401db-42e9-4f5b-a7dd-0e2a6af555be</TermId>
-        </TermInfo>
-      </Terms>
-    </nb1b8a72855341e18dd75ce464e281f2>
-    <eDocs_eFileName xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">ENT218-001-2023</eDocs_eFileName>
-    <mbbd3fafa5ab4e5eb8a6a5e099cef439 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Unclassified</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">779752a3-a421-4077-839c-91815f544ae2</TermId>
-        </TermInfo>
-      </Terms>
-    </mbbd3fafa5ab4e5eb8a6a5e099cef439>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="eDocument" ma:contentTypeID="0x0101000BC94875665D404BB1351B53C41FD2C000E5CBA74D75A77049B177D97877D56E03" ma:contentTypeVersion="181" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9aef13b51d858ac71ab25d278c7edb31">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f94102a1-1d6c-4502-ac27-91905b9321dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="992d5dd0ba35d17e896caa4d336a12f8" ns2:_="">
     <xsd:import namespace="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
@@ -1277,6 +1221,45 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <m02c691f3efa402dab5cbaa8c240a9e7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m02c691f3efa402dab5cbaa8c240a9e7>
+    <TaxCatchAll xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Value>5</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <eDocs_FileStatus xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">Live</eDocs_FileStatus>
+    <h1f8bb4843d6459a8b809123185593c7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">218</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d1f665d0-1ea2-48c4-9fae-9dfb881d0110</TermId>
+        </TermInfo>
+      </Terms>
+    </h1f8bb4843d6459a8b809123185593c7>
+    <fbaa881fc4ae443f9fdafbdd527793df xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </fbaa881fc4ae443f9fdafbdd527793df>
+    <_vti_ItemDeclaredRecord xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd" xsi:nil="true"/>
+    <nb1b8a72855341e18dd75ce464e281f2 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </nb1b8a72855341e18dd75ce464e281f2>
+    <eDocs_eFileName xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd" xsi:nil="true"/>
+    <mbbd3fafa5ab4e5eb8a6a5e099cef439 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Unclassified</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">779752a3-a421-4077-839c-91815f544ae2</TermId>
+        </TermInfo>
+      </Terms>
+    </mbbd3fafa5ab4e5eb8a6a5e099cef439>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1287,23 +1270,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A59B2-55CF-4E9A-ADEC-6D1F626366C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3707964B-8A63-4BFC-AE72-47FB7628B095}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8906BC1-B9F8-468F-B62B-D526A3815BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1320,8 +1287,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9E62FD8-E82F-4E04-9CFE-AF6725E34E21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630F9CF-D4FF-4CEA-98D4-56CE26D676B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED1DE1DA-BB70-4DB0-810A-3DCE6B3A632C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>

</xml_diff>